<commit_message>
Project Completion by sending mail 08/Sep/2022
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\syste\OneDrive\Documents\UiPath\RE Framework\Daily Fun Fact_Daily English\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68E5ED84-7943-4FA9-889A-1B09767D70D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46CCE94E-C7C2-4B08-AFF0-4A694BB7273E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="68">
   <si>
     <t>Name</t>
   </si>
@@ -95,96 +95,146 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
+    <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction succesful.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction failed with business exception.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction failed with application exception.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Calling Get Transaction Data.</t>
+  </si>
+  <si>
+    <t>OrchestratorAssetFolder</t>
+  </si>
+  <si>
+    <t>OrchestratorQueueFolder</t>
+  </si>
+  <si>
+    <t>Folder name. The value must match a folder defined in Orchestrator and queue specified as OrchestratorQueueName should be created in this folder. For classic folders leave the value field empty.</t>
+  </si>
+  <si>
+    <t>MaxConsecutiveSystemExceptions</t>
+  </si>
+  <si>
+    <t>ExceptionMessage_ConsecutiveErrors</t>
+  </si>
+  <si>
+    <t>RetryNumberGetTransactionItem</t>
+  </si>
+  <si>
+    <t>RetryNumberSetTransactionStatus</t>
+  </si>
+  <si>
+    <t>Error message in case MaxConsecutiveSystemExceptions number is reached.</t>
+  </si>
+  <si>
+    <t>The number of times Get Transaction Item activity is retried in case of an exception. Must be an integer &gt;= 1.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of times Set transaction status activity is retried in case of an exception. Must be an integer &gt;= 1. </t>
+  </si>
+  <si>
+    <t>ShouldMarkJobAsFaulted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of consecutive system exceptions allowed. If MaxConsecutiveSystemExceptions is reached, the job is stopped. To disable this feature, set the value to 0. </t>
+  </si>
+  <si>
+    <t>Must be TRUE or FALSE. If the value is TRUE and an error occurs in Initialization state or the MaxConsecutiveSystemExceptions is reached, the job is marked as Faulted.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
+  </si>
+  <si>
+    <t>Daily English</t>
+  </si>
+  <si>
+    <t>Daily Fun Fact - Daily English</t>
+  </si>
+  <si>
+    <t>https://www.englishtohindisentences.com/2022/01/17/daily-use-english-to-tamil-sentences/</t>
+  </si>
+  <si>
+    <t>EnglishToTamilSentenceInputExcelPath</t>
+  </si>
+  <si>
+    <t>C:\Users\syste\OneDrive\Documents\UiPath\RE Framework\Daily Fun Fact_Daily English\Data\Input\English and Tamil Sentences.xlsx</t>
+  </si>
+  <si>
+    <t>This excel contains 5000 english and tamil sentences which is extracted from the website</t>
+  </si>
+  <si>
     <t>OrchestratorQueueName</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction succesful.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction failed with business exception.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction failed with application exception.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Calling Get Transaction Data.</t>
-  </si>
-  <si>
-    <t>OrchestratorAssetFolder</t>
-  </si>
-  <si>
-    <t>OrchestratorQueueFolder</t>
-  </si>
-  <si>
-    <t>Folder name. The value must match a folder defined in Orchestrator and queue specified as OrchestratorQueueName should be created in this folder. For classic folders leave the value field empty.</t>
-  </si>
-  <si>
-    <t>MaxConsecutiveSystemExceptions</t>
-  </si>
-  <si>
-    <t>ExceptionMessage_ConsecutiveErrors</t>
-  </si>
-  <si>
-    <t>RetryNumberGetTransactionItem</t>
-  </si>
-  <si>
-    <t>RetryNumberSetTransactionStatus</t>
-  </si>
-  <si>
-    <t>Error message in case MaxConsecutiveSystemExceptions number is reached.</t>
-  </si>
-  <si>
-    <t>The number of times Get Transaction Item activity is retried in case of an exception. Must be an integer &gt;= 1.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of times Set transaction status activity is retried in case of an exception. Must be an integer &gt;= 1. </t>
-  </si>
-  <si>
-    <t>ShouldMarkJobAsFaulted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of consecutive system exceptions allowed. If MaxConsecutiveSystemExceptions is reached, the job is stopped. To disable this feature, set the value to 0. </t>
-  </si>
-  <si>
-    <t>Must be TRUE or FALSE. If the value is TRUE and an error occurs in Initialization state or the MaxConsecutiveSystemExceptions is reached, the job is marked as Faulted.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
-  </si>
-  <si>
-    <t>Daily English</t>
-  </si>
-  <si>
-    <t>Daily Fun Fact - Daily English</t>
-  </si>
-  <si>
-    <t>EnglishToTamilSentenceUrl</t>
-  </si>
-  <si>
-    <t>https://www.englishtohindisentences.com/2022/01/17/daily-use-english-to-tamil-sentences/</t>
-  </si>
-  <si>
-    <t>5000 English and Tamil Sentences Website open url</t>
-  </si>
-  <si>
-    <t>EnglishToTamilSentenceInputExcelPath</t>
-  </si>
-  <si>
-    <t>C:\Users\syste\OneDrive\Documents\UiPath\RE Framework\Daily Fun Fact_Daily English\Data\Input\English and Tamil Sentences.xlsx</t>
-  </si>
-  <si>
-    <t>This excel contains 5000 english and tamil sentences which is extracted from the website</t>
+  </si>
+  <si>
+    <t>DailyFunFactWebsiteUrl</t>
+  </si>
+  <si>
+    <t>https://www.beagreatteacher.com/daily-fun-fact/</t>
+  </si>
+  <si>
+    <t>Daily Fun Fact website url</t>
+  </si>
+  <si>
+    <t>EnglishTamilSentencesPageUrl</t>
+  </si>
+  <si>
+    <t>MailToAddress</t>
+  </si>
+  <si>
+    <t>MailSubject</t>
+  </si>
+  <si>
+    <t>MailBody</t>
+  </si>
+  <si>
+    <t>5000 english and tamil sentences website open url</t>
+  </si>
+  <si>
+    <t>mail to address</t>
+  </si>
+  <si>
+    <t>mail body</t>
+  </si>
+  <si>
+    <t>MailPortNumber</t>
+  </si>
+  <si>
+    <t>MailServerName</t>
+  </si>
+  <si>
+    <t>Mail Port Number</t>
+  </si>
+  <si>
+    <t>EmailAssetName</t>
+  </si>
+  <si>
+    <t>Mail Server Name</t>
+  </si>
+  <si>
+    <t>Email Credentials</t>
+  </si>
+  <si>
+    <t>Mail Login Credentials</t>
+  </si>
+  <si>
+    <t>smtp.gmail.com</t>
+  </si>
+  <si>
+    <t>sankaravenie5@gmail.com;sathyamoorthie5@gmail.com;sharongiftae5@gmail.com;aartiak.e5@gmail.com;sornalakshmie5@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -208,6 +258,19 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF464E55"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -226,10 +289,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -239,8 +303,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -553,16 +625,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z998"/>
+  <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="43.54296875" customWidth="1"/>
-    <col min="2" max="2" width="45.08984375" customWidth="1"/>
+    <col min="2" max="2" width="52.36328125" customWidth="1"/>
     <col min="3" max="3" width="81.453125" customWidth="1"/>
     <col min="4" max="26" width="8.6328125" customWidth="1"/>
   </cols>
@@ -603,10 +675,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -614,11 +686,11 @@
     </row>
     <row r="3" spans="1:26" ht="43.5">
       <c r="A3" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -627,43 +699,107 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="30" customHeight="1">
+    <row r="7" spans="1:26" ht="47" customHeight="1">
       <c r="A7" t="s">
         <v>45</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="32" customHeight="1">
+    <row r="8" spans="1:26" ht="24" customHeight="1">
       <c r="A8" t="s">
-        <v>48</v>
-      </c>
-      <c r="B8" s="3" t="s">
         <v>49</v>
       </c>
+      <c r="B8" t="s">
+        <v>50</v>
+      </c>
       <c r="C8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:26" ht="33.5" customHeight="1">
+      <c r="A9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="47.5" customHeight="1">
+      <c r="A10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="6">
+        <v>465</v>
+      </c>
+      <c r="C13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="18" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
     <row r="19" ht="14.25" customHeight="1"/>
@@ -1645,11 +1781,13 @@
     <row r="995" ht="14.25" customHeight="1"/>
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
-    <row r="998" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
+  <hyperlinks>
+    <hyperlink ref="B9" r:id="rId1" xr:uid="{E653F4C1-33BF-4449-B3A0-8BF780F92183}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1711,18 +1849,18 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="43.5">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1746,7 +1884,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -1768,7 +1906,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1779,7 +1917,7 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
@@ -1790,53 +1928,53 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" spans="1:3" ht="29">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B17" t="b">
         <v>1</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2840,7 +2978,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
reference number updated 08/sep/2022 12.21 pm
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\syste\OneDrive\Documents\UiPath\RE Framework\Daily Fun Fact_Daily English\Data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46CCE94E-C7C2-4B08-AFF0-4A694BB7273E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10305"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -164,9 +158,6 @@
     <t>EnglishToTamilSentenceInputExcelPath</t>
   </si>
   <si>
-    <t>C:\Users\syste\OneDrive\Documents\UiPath\RE Framework\Daily Fun Fact_Daily English\Data\Input\English and Tamil Sentences.xlsx</t>
-  </si>
-  <si>
     <t>This excel contains 5000 english and tamil sentences which is extracted from the website</t>
   </si>
   <si>
@@ -227,13 +218,16 @@
     <t>smtp.gmail.com</t>
   </si>
   <si>
-    <t>sankaravenie5@gmail.com;sathyamoorthie5@gmail.com;sharongiftae5@gmail.com;aartiak.e5@gmail.com;sornalakshmie5@gmail.com</t>
+    <t>sankaravenie5@gmail.com;sathyamoorthie5@gmail.com;sharongiftae5@gmail.com;aartiak.e5@gmail.com;sornalakshmie5@gmail.com;naresh.kumar@e5.ai;lakshmi.u@tiliconveli.com;narenbagavathye5@gmail.com;prasanth9534@gmail.com</t>
+  </si>
+  <si>
+    <t>\Data\Input\English and Tamil Sentences.xlsx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6">
     <font>
       <sz val="11"/>
@@ -245,6 +239,7 @@
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="6"/>
@@ -263,6 +258,7 @@
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -371,7 +367,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -423,7 +419,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -617,26 +613,26 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.54296875" customWidth="1"/>
-    <col min="2" max="2" width="52.36328125" customWidth="1"/>
-    <col min="3" max="3" width="81.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.6328125" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="2" max="2" width="52.42578125" customWidth="1"/>
+    <col min="3" max="3" width="81.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -675,7 +671,7 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>42</v>
@@ -684,7 +680,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.5">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" s="2" t="s">
         <v>29</v>
       </c>
@@ -694,7 +690,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="29">
+    <row r="5" spans="1:26" ht="30">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -706,97 +702,97 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="47" customHeight="1">
+    <row r="7" spans="1:26" ht="47.1" customHeight="1">
       <c r="A7" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" t="s">
         <v>46</v>
-      </c>
-      <c r="C7" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="24" customHeight="1">
       <c r="A8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" t="s">
         <v>49</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>50</v>
       </c>
-      <c r="C8" t="s">
+    </row>
+    <row r="9" spans="1:26" ht="33.6" customHeight="1">
+      <c r="A9" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="33.5" customHeight="1">
-      <c r="A9" t="s">
-        <v>52</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>44</v>
       </c>
       <c r="C9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="47.45" customHeight="1">
+      <c r="A10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" t="s">
         <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" ht="47.5" customHeight="1">
-      <c r="A10" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C10" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B11" t="s">
         <v>43</v>
       </c>
       <c r="C11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B13" s="6">
         <v>465</v>
       </c>
       <c r="C13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B15" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="18" customHeight="1"/>
@@ -1784,7 +1780,7 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <hyperlinks>
-    <hyperlink ref="B9" r:id="rId1" xr:uid="{E653F4C1-33BF-4449-B3A0-8BF780F92183}"/>
+    <hyperlink ref="B9" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -1792,19 +1788,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.6328125" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1841,7 +1837,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="29">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1852,7 +1848,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.5">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -1966,7 +1962,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="29">
+    <row r="17" spans="1:3" ht="45">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -2955,19 +2951,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.90625" customWidth="1"/>
-    <col min="2" max="2" width="30.08984375" customWidth="1"/>
-    <col min="3" max="3" width="60.36328125" customWidth="1"/>
-    <col min="4" max="26" width="65.453125" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="60.42578125" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>